<commit_message>
Added A02 - Project Exploration
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -5,29 +5,40 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C1325D-E7E3-2B49-910D-EE9F746C44A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8FD821-5BA6-6644-82A8-D61E46FC2708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAE" sheetId="1" r:id="rId1"/>
     <sheet name="Homework" sheetId="11" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="22" r:id="rId3"/>
-    <sheet name="Blog" sheetId="3" r:id="rId4"/>
-    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId5"/>
-    <sheet name="ProjectCheckpoint" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="23" r:id="rId7"/>
-    <sheet name="Poster" sheetId="21" r:id="rId8"/>
-    <sheet name="CodeReview" sheetId="19" r:id="rId9"/>
-    <sheet name="Discussion" sheetId="18" r:id="rId10"/>
-    <sheet name="ProjectReport" sheetId="15" r:id="rId11"/>
-    <sheet name="ResearchReport" sheetId="17" r:id="rId12"/>
+    <sheet name="ProjExploration" sheetId="24" r:id="rId3"/>
+    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId5"/>
+    <sheet name="Blog" sheetId="3" r:id="rId6"/>
+    <sheet name="ProjectCheckpoint" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId8"/>
+    <sheet name="Poster" sheetId="21" r:id="rId9"/>
+    <sheet name="CodeReview" sheetId="19" r:id="rId10"/>
+    <sheet name="Discussion" sheetId="18" r:id="rId11"/>
+    <sheet name="ProjectReport" sheetId="15" r:id="rId12"/>
+    <sheet name="ResearchReport" sheetId="17" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="215">
   <si>
     <t>Score</t>
   </si>
@@ -2115,6 +2126,21 @@
   </si>
   <si>
     <t>On time; Fails to fully address all parts of the assignment; work demonstrates a lack of effort, care and/or understanding; disorganized, sloppy or hard to understand.</t>
+  </si>
+  <si>
+    <t>Homework</t>
+  </si>
+  <si>
+    <t>On time; All explorations contain all required information;  Information presented gives a thoughful, clear and detailed picture of the projects; Writing is clear, concise, well organized, uses complete senteces and proper grammar; Explorations are correctly linked, neatly formatted and easy to read.</t>
+  </si>
+  <si>
+    <t>On time; All explorations contain all required information; Information presented accurately describes the project; Writing may have minor issues but does not distract from meaning or understanding; Explorations are correctly linked but may be poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>On time; One or more exploratiions may be missing entirely or missing required information; Information in the exploration does not give an adequate picture of the project; Information may simply be copy and pasted; Writing, formatting or grammar may interfear with understanding. Explorations may be incorrectly linked, poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>Late, missing or substantially incomplete; clearly demonstrates little to no investment in the assignment.</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2186,6 +2212,27 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2499,7 +2546,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2585,6 +2632,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="112">
@@ -3148,6 +3222,95 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="5" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:5" ht="17" thickBot="1"/>
+    <row r="3" spans="3:5" ht="17" thickBot="1">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" ht="34">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="102">
+      <c r="C5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="68">
+      <c r="C6" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="86" thickBot="1">
+      <c r="C7" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="68">
+      <c r="D10" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="D11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:G11"/>
   <sheetViews>
@@ -3268,7 +3431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C10:H16"/>
   <sheetViews>
@@ -3414,7 +3577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="C10:G16"/>
   <sheetViews>
@@ -3546,8 +3709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C2:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3557,7 +3720,11 @@
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="17" thickBot="1"/>
+    <row r="2" spans="3:4" ht="17" thickBot="1">
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="3" spans="3:4" ht="17" thickBot="1">
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -3610,6 +3777,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
+  <dimension ref="C2:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="17" thickBot="1"/>
+    <row r="3" spans="3:6" ht="17" thickBot="1">
+      <c r="C3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" ht="102">
+      <c r="C4" s="36">
+        <v>3</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="3:6" ht="102">
+      <c r="C5" s="34">
+        <v>2</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="3:6" ht="119">
+      <c r="C6" s="34">
+        <v>1</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="35" thickBot="1">
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="D3:H16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="9" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:8" ht="17" thickBot="1"/>
+    <row r="4" spans="4:8" ht="17" thickBot="1">
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" ht="51">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" ht="103" thickBot="1">
+      <c r="D6" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="102">
+      <c r="D7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="69" thickBot="1">
+      <c r="D8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" ht="17" thickBot="1"/>
+    <row r="12" spans="4:8" ht="17" thickBot="1">
+      <c r="D12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" ht="51">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" ht="86" thickBot="1">
+      <c r="D14" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" ht="102">
+      <c r="D15" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" ht="69" thickBot="1">
+      <c r="D16" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB29A2B-D501-E842-859E-32CF9B172168}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3621,7 +4049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C2:G11"/>
   <sheetViews>
@@ -3745,204 +4173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="D3:H16"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="9" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="4:8" ht="17" thickBot="1"/>
-    <row r="4" spans="4:8" ht="17" thickBot="1">
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="4:8" ht="51">
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="4:8" ht="103" thickBot="1">
-      <c r="D6" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" ht="102">
-      <c r="D7" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" ht="69" thickBot="1">
-      <c r="D8" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="4:8" ht="17" thickBot="1"/>
-    <row r="12" spans="4:8" ht="17" thickBot="1">
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="4:8" ht="51">
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="4:8" ht="86" thickBot="1">
-      <c r="D14" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="4:8" ht="102">
-      <c r="D15" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="4:8" ht="69" thickBot="1">
-      <c r="D16" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C2:I7"/>
   <sheetViews>
@@ -4083,7 +4314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B90E7E3-D2D8-464A-A6B2-25D7F2B455CA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4095,7 +4326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:H10"/>
   <sheetViews>
@@ -4230,93 +4461,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="5" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:5" ht="17" thickBot="1"/>
-    <row r="3" spans="3:5" ht="17" thickBot="1">
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" ht="34">
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="102">
-      <c r="C5" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" ht="68">
-      <c r="C6" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" ht="86" thickBot="1">
-      <c r="C7" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" ht="68">
-      <c r="D10" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5">
-      <c r="D11" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated proj rev rubric
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0006D649-FF51-0449-B83C-A84B6175B897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A6565A-1C2C-734A-AD5B-8FC310E9DD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2140,19 +2140,19 @@
     <t>Project Review</t>
   </si>
   <si>
-    <t>On time; All reviews contain all required information; Information presented accurately describes the project; Writing may have minor issues but does not distract from meaning or understanding; Reviews are correctly linked but may be poorly formatted or difficult to read.</t>
-  </si>
-  <si>
     <t>On time; One or more exploratiions may be missing entirely or missing required information; Information in the exploration does not give an adequate picture of the project; Information may simply be copy and pasted; Writing, formatting or grammar may interfear with understanding; Explorations may be incorrectly linked, poorly formatted or difficult to read.</t>
   </si>
   <si>
-    <t>On time; One or more reviews may be missing entirely or missing required information; Information in the exploration does not give an adequate picture of the project; Information may simply be copy and pasted; Writing, formatting or grammar may interfear with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
-  </si>
-  <si>
     <t>Late, missing or substantially incomplete; Clearly demonstrates little to no investment in the assignment.</t>
   </si>
   <si>
-    <t>On time; All reviews contain all required information;  Information presented gives a thoughful, clear and highly detailed picture of the projects; Writing is clear, concise, well organized, uses complete senteces and proper grammar; Reviews are correctly linked, neatly formatted and easy to read.</t>
+    <t>On time; All reviews contain all required information; Information presented addresses the prompts; Summaries of each section are largely factual rather than reflective; Writing may have minor issues but does not distract from meaning or understanding; Reviews are correctly linked but may be poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>On time; All reviews contain all required information;  Information presented gives a clear and highly detailed picture of the projects; Summaries of each section are thoughtful, reflective and insightful; Writing is clear, concise, well organized, uses complete sentences and proper grammar; Reviews are correctly linked, neatly formatted and easy to read.</t>
+  </si>
+  <si>
+    <t>On time; One or more reviews may be missing entirely or missing required information; Information in the review does not give an adequate picture of the project; Summaries of each section are cursory or do not align with the review; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
   </si>
 </sst>
 </file>
@@ -3792,8 +3792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
   <dimension ref="C2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D14"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3835,7 +3835,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="35" thickBot="1">
@@ -3843,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="17" thickBot="1"/>
@@ -3855,20 +3855,20 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="3:6" ht="102">
+    <row r="11" spans="3:6" ht="119">
       <c r="C11" s="36">
         <v>3</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="85">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="119">
       <c r="C12" s="34">
         <v>2</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="3:6" ht="119">
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="35" thickBot="1">
@@ -3884,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added A02c for Project Ranking and Selection
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A6565A-1C2C-734A-AD5B-8FC310E9DD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB944E8-94AF-A241-BC7F-5CC124A37DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="-20760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAE" sheetId="1" r:id="rId1"/>
     <sheet name="Homework" sheetId="11" r:id="rId2"/>
-    <sheet name="ProjExploration" sheetId="24" r:id="rId3"/>
+    <sheet name="ProjSelection" sheetId="24" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="22" r:id="rId4"/>
     <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId5"/>
     <sheet name="Blog" sheetId="3" r:id="rId6"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="223">
   <si>
     <t>Score</t>
   </si>
@@ -2153,6 +2153,18 @@
   </si>
   <si>
     <t>On time; One or more reviews may be missing entirely or missing required information; Information in the review does not give an adequate picture of the project; Summaries of each section are cursory or do not align with the review; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>Project Ranking and Selection</t>
+  </si>
+  <si>
+    <t>On time; Wiki contains all required information;  Information presented gives a clear and highly detailed picture of why the team selected the project that they did; Rankings and selection are clearly and well supported by thoughtful, reflective and insightful rationales that draw directly on the gathered information; Writing is clear, concise, well organized, uses complete sentences and proper grammar; Wiki is correctly linked, neatly formatted and easy to read.</t>
+  </si>
+  <si>
+    <t>On time; Wiki contains all required information; Information presented indicates why the team selected the project that they did; Rankings and selection are supported by rationales that mention gathered information; Writing may have minor issues but does not distract from meaning or understanding; Reviews are correctly linked but may be poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>On time; Wiki may be missing required information; Information in the Wiki does not give an adequate picture of why the team selected the project they did; Rankings may be insufficiently connected to the rationale or rationale may not use or may not align with provided information; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
   </si>
 </sst>
 </file>
@@ -3790,10 +3802,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
-  <dimension ref="C2:F14"/>
+  <dimension ref="C2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3884,6 +3896,47 @@
         <v>0</v>
       </c>
       <c r="D14" s="35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="17" thickBot="1"/>
+    <row r="21" spans="3:4" ht="17" thickBot="1">
+      <c r="C21" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="153">
+      <c r="C22" s="36">
+        <v>3</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="116" customHeight="1">
+      <c r="C23" s="34">
+        <v>2</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="132" customHeight="1">
+      <c r="C24" s="34">
+        <v>1</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="35" thickBot="1">
+      <c r="C25" s="33">
+        <v>0</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>215</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added A03 for Blog Post
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB944E8-94AF-A241-BC7F-5CC124A37DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B097532-041E-E246-A897-6315B702CBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="-20760" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1220" yWindow="-18640" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAE" sheetId="1" r:id="rId1"/>
     <sheet name="Homework" sheetId="11" r:id="rId2"/>
     <sheet name="ProjSelection" sheetId="24" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="22" r:id="rId4"/>
-    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId5"/>
-    <sheet name="Blog" sheetId="3" r:id="rId6"/>
+    <sheet name="Blog" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId5"/>
+    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId6"/>
     <sheet name="ProjectCheckpoint" sheetId="4" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="23" r:id="rId8"/>
     <sheet name="Poster" sheetId="21" r:id="rId9"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="228">
   <si>
     <t>Score</t>
   </si>
@@ -1443,9 +1443,6 @@
     <t>One or more posts were absent or trivial at the time of assessment.</t>
   </si>
   <si>
-    <t>All blog posts were made on time.</t>
-  </si>
-  <si>
     <t>Blog posts were trivial at the time of assessment.</t>
   </si>
   <si>
@@ -2165,6 +2162,24 @@
   </si>
   <si>
     <t>On time; Wiki may be missing required information; Information in the Wiki does not give an adequate picture of why the team selected the project they did; Rankings may be insufficiently connected to the rationale or rationale may not use or may not align with provided information; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
+  </si>
+  <si>
+    <t>Blog posts were made on time.</t>
+  </si>
+  <si>
+    <t>Critera</t>
+  </si>
+  <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>On time; Post has a thesis that is insightful or will be thought provking and is clearly connected to a course topic; Text integrates readings, discussion and/or other sources; Writing is well organized, gramatically correct. Post is likely to be of interest to an external audience; Links and use of media are integrated and enhance the post; Post is of appropriate length.</t>
+  </si>
+  <si>
+    <t>On time; Post has a recognizable thesis and is  connected to a course topic; Text touches on readings, discussion and/or other sources; Writing contains few grammatical errors that do not interfere with meaning; Post may be contextualized in the course, potentially limiting interest to an external audience; Links and use of media may not be fully integrated; Post may be slightly short or long.</t>
+  </si>
+  <si>
+    <t>On time; Post lacks a thesis and/or is not clearly connected to a course topic; Text does not draw on readings, discussion and/or other sources; Writing is disorganized and/or contains grammatical errors that interfere with meaning; Links and/or use of media seem disconnected or gratuitious; Post is excessively short or long.</t>
   </si>
 </sst>
 </file>
@@ -2570,7 +2585,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2596,7 +2611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13"/>
@@ -2636,9 +2651,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2654,7 +2666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2681,7 +2693,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3147,17 +3159,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="17" thickBot="1">
-      <c r="D2" s="29"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="3:7" ht="17" thickBot="1">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
@@ -3167,20 +3179,20 @@
       </c>
     </row>
     <row r="4" spans="3:7" ht="170">
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>3</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>200</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>191</v>
+        <v>149</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="102">
@@ -3188,16 +3200,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>202</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="119">
@@ -3205,33 +3217,33 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="86" thickBot="1">
+      <c r="C7" s="27">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="86" thickBot="1">
-      <c r="C7" s="28">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>204</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3265,10 +3277,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="34">
@@ -3276,21 +3288,21 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="5" spans="3:5" ht="102">
-      <c r="C5" s="23" t="s">
-        <v>134</v>
+      <c r="C5" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="68">
@@ -3298,10 +3310,10 @@
         <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="86" thickBot="1">
@@ -3309,15 +3321,15 @@
         <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="68">
       <c r="D10" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="3:5">
@@ -3354,16 +3366,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="3:7" ht="34">
@@ -3371,33 +3383,33 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="120" thickBot="1">
       <c r="C5" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="102">
@@ -3405,16 +3417,16 @@
         <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="69" thickBot="1">
@@ -3422,21 +3434,21 @@
         <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="102">
       <c r="D10" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="9"/>
     </row>
@@ -3746,7 +3758,7 @@
   <sheetData>
     <row r="2" spans="3:4" ht="17" thickBot="1">
       <c r="C2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="17" thickBot="1">
@@ -3762,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="51">
@@ -3770,15 +3782,15 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="68">
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="35" thickBot="1">
@@ -3786,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3804,8 +3816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
   <dimension ref="C2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3817,127 +3829,127 @@
   <sheetData>
     <row r="2" spans="3:6" ht="17" thickBot="1"/>
     <row r="3" spans="3:6" ht="17" thickBot="1">
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="3:6" ht="102">
-      <c r="C4" s="36">
+      <c r="C4" s="35">
         <v>3</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="3:6" ht="102">
+      <c r="C5" s="33">
+        <v>2</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="38"/>
-    </row>
-    <row r="5" spans="3:6" ht="102">
-      <c r="C5" s="34">
-        <v>2</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="F5" s="38"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="3:6" ht="119">
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>1</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="52" thickBot="1">
+      <c r="C7" s="32">
+        <v>0</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" ht="35" thickBot="1">
-      <c r="C7" s="33">
-        <v>0</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="17" thickBot="1"/>
     <row r="10" spans="3:6" ht="17" thickBot="1">
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>213</v>
+      <c r="D10" s="30" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="119">
-      <c r="C11" s="36">
+      <c r="C11" s="35">
         <v>3</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="119">
+      <c r="C12" s="33">
+        <v>2</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="136">
+      <c r="C13" s="33">
+        <v>1</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="3:6" ht="119">
-      <c r="C12" s="34">
-        <v>2</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" ht="119">
-      <c r="C13" s="34">
-        <v>1</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" ht="35" thickBot="1">
-      <c r="C14" s="33">
+    <row r="14" spans="3:6" ht="52" thickBot="1">
+      <c r="C14" s="32">
         <v>0</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>215</v>
+      <c r="D14" s="34" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="17" thickBot="1"/>
     <row r="21" spans="3:4" ht="17" thickBot="1">
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="153">
+      <c r="C22" s="35">
+        <v>3</v>
+      </c>
+      <c r="D22" s="36" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="153">
-      <c r="C22" s="36">
-        <v>3</v>
-      </c>
-      <c r="D22" s="37" t="s">
+    <row r="23" spans="3:4" ht="116" customHeight="1">
+      <c r="C23" s="33">
+        <v>2</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="116" customHeight="1">
-      <c r="C23" s="34">
-        <v>2</v>
-      </c>
-      <c r="D23" s="32" t="s">
+    <row r="24" spans="3:4" ht="132" customHeight="1">
+      <c r="C24" s="33">
+        <v>1</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="132" customHeight="1">
-      <c r="C24" s="34">
-        <v>1</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" ht="35" thickBot="1">
-      <c r="C25" s="33">
+    <row r="25" spans="3:4" ht="52" thickBot="1">
+      <c r="C25" s="32">
         <v>0</v>
       </c>
-      <c r="D25" s="35" t="s">
-        <v>215</v>
+      <c r="D25" s="34" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3947,6 +3959,214 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="12" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="17" thickBot="1"/>
+    <row r="2" spans="2:12" ht="17" thickBot="1">
+      <c r="B2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="137" thickBot="1">
+      <c r="B3" s="35">
+        <v>3</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="154" thickBot="1">
+      <c r="B4" s="33">
+        <v>2</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="121" customHeight="1">
+      <c r="B5" s="33">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="52" thickBot="1">
+      <c r="B6" s="32">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="17" customHeight="1"/>
+    <row r="9" spans="2:12" ht="17" thickBot="1"/>
+    <row r="10" spans="2:12" ht="17" thickBot="1">
+      <c r="H10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="103" thickBot="1">
+      <c r="H11" s="22">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="102">
+      <c r="H12" s="21">
+        <v>2</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="86" thickBot="1">
+      <c r="H13" s="22">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="51">
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="85">
+      <c r="I16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9">
+      <c r="I17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" ht="17" thickBot="1"/>
+    <row r="21" spans="8:9" ht="17" thickBot="1">
+      <c r="H21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="8:9" ht="18" thickBot="1">
+      <c r="H22" s="22">
+        <v>3</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9" ht="17">
+      <c r="H23" s="21">
+        <v>2</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" ht="18" thickBot="1">
+      <c r="H24" s="22">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" ht="34">
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I17" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB29A2B-D501-E842-859E-32CF9B172168}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3958,7 +4178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="D3:H16"/>
   <sheetViews>
@@ -4009,7 +4229,7 @@
     </row>
     <row r="6" spans="4:8" ht="103" thickBot="1">
       <c r="D6" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>32</v>
@@ -4021,7 +4241,7 @@
         <v>34</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="4:8" ht="102">
@@ -4038,7 +4258,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="4:8" ht="69" thickBot="1">
@@ -4087,7 +4307,7 @@
         <v>27</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>25</v>
@@ -4095,7 +4315,7 @@
     </row>
     <row r="14" spans="4:8" ht="86" thickBot="1">
       <c r="D14" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>28</v>
@@ -4104,10 +4324,10 @@
         <v>29</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="4:8" ht="102">
@@ -4121,10 +4341,10 @@
         <v>24</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="4:8" ht="69" thickBot="1">
@@ -4145,130 +4365,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="C2:G11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="7" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:7" ht="17" thickBot="1"/>
-    <row r="3" spans="3:7" ht="17" thickBot="1">
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" ht="51">
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="86" thickBot="1">
-      <c r="C5" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="102">
-      <c r="C6" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="103" thickBot="1">
-      <c r="C7" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="85">
-      <c r="D10" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7">
-      <c r="D11" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -4302,16 +4398,16 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>36</v>
@@ -4325,16 +4421,16 @@
         <v>39</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>25</v>
@@ -4342,22 +4438,22 @@
     </row>
     <row r="5" spans="3:9" ht="103" thickBot="1">
       <c r="C5" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>42</v>
@@ -4368,13 +4464,13 @@
         <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>37</v>
@@ -4394,10 +4490,10 @@
         <v>89</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>90</v>
@@ -4455,19 +4551,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="68">
@@ -4475,39 +4571,39 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="117" customHeight="1">
+      <c r="C5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" ht="117" customHeight="1">
-      <c r="C5" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="102">
@@ -4515,19 +4611,19 @@
         <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="69" thickBot="1">
@@ -4541,18 +4637,18 @@
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="119">
       <c r="E9" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="3:8">

</xml_diff>

<commit_message>
Added Project Selection presentation info to A02c
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B097532-041E-E246-A897-6315B702CBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C021A85-0D71-A943-A486-5A3DF12CAEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1220" yWindow="-18640" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3200" yWindow="-21040" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAE" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="214">
   <si>
     <t>Score</t>
   </si>
@@ -67,27 +67,9 @@
     <t>Writing</t>
   </si>
   <si>
-    <t>Mechanics</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
     <t>Note: Some langauge adapted from http://foss2serve.org/index.php/FOSS_Course_Syllabus#2._Methods_of_Assessment</t>
   </si>
   <si>
-    <t>This work is licensed under a Creative Commons Attribution-ShareAlike 4.0 International License</t>
-  </si>
-  <si>
-    <t>Blog post is of appropriate length, contains few (if any) grammatical errors, and multimedia use (if any) is appropriate.</t>
-  </si>
-  <si>
-    <t>Timeliness</t>
-  </si>
-  <si>
-    <t>Blog post is excessively short or long, writing contains significant grammatical errors and/or multimedia use is gratuitous.</t>
-  </si>
-  <si>
     <t>Completion</t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>The team/sub-team accomplishments were not summarized.</t>
   </si>
   <si>
-    <t>Writing is disorganized, drab,  and/or uninteresting.</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -1440,18 +1419,6 @@
     </r>
   </si>
   <si>
-    <t>One or more posts were absent or trivial at the time of assessment.</t>
-  </si>
-  <si>
-    <t>Blog posts were trivial at the time of assessment.</t>
-  </si>
-  <si>
-    <t>Writing is largely incoherent.</t>
-  </si>
-  <si>
-    <t>Content has no discernable connection to the reading/discussion topic.</t>
-  </si>
-  <si>
     <t>Note: Some langauge adapted from http://users.dickinson.edu/~jmac/courses/spring-2017-comp492/assignments/A2-discussion-v1.pdf</t>
   </si>
   <si>
@@ -1846,11 +1813,57 @@
     <t>Attended class but may have been late and/or left the room with unusual frequency or duration..</t>
   </si>
   <si>
-    <t>Writing is clear, concise, and interesting.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Writing is </t>
+    <t>Presentation was engaging, clearly conveyed the project information, used media effectively, allowed equal participation by team members and was an appropriate length.</t>
+  </si>
+  <si>
+    <t>Presentation was not engaging, unclear, incomplete, excessively long or short, used media gratuitously or ineffectively and/or did not balance presentation among team members.</t>
+  </si>
+  <si>
+    <t>Presentation was not engaging, unclear, incomplete, excessively long or short and/or used media gratuitously or ineffectively.</t>
+  </si>
+  <si>
+    <t>Presentation engaging, used media effectively, clearly conveyed the aim, context and plan for the proposed research in an appropriate amount of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposal was not submitted or is missing significant required content.  </t>
+  </si>
+  <si>
+    <t>The proposal is insufficient and/or unclear in its presentation of the research question and/or literature survey and/or research plan.</t>
+  </si>
+  <si>
+    <t>Proposal clearly states the research question and contextualizes it within the relevant literature and proposes a viable research plan for answering the question..</t>
+  </si>
+  <si>
+    <t>Readings</t>
+  </si>
+  <si>
+    <t>Questions were submitted late, show little thought, miss significant issues, limit or presuppose perspectives or are unlikely to lead to interesting discussion.</t>
+  </si>
+  <si>
+    <t>Questions are thoughtful, probe at the important issues, are open to multiple perspectives  and seem likely to generate interesting discussion.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Questions clearly meet criterion for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Lucida Grande"/>
+        <family val="2"/>
+      </rPr>
+      <t>✓</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1861,59 +1874,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>exceptionally</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve"> well organized and interesting.</t>
-    </r>
-  </si>
-  <si>
-    <t>Content is insufficiently connected to the topic and/or demonstrates unfamiliarity with or misunderstanding of the topic and/or is simply a class summary.</t>
-  </si>
-  <si>
-    <t>Content is clearly connected to the topic, demonstrates that the reading and discussion were reflected upon, has a clear focus of broad interest and provides personal insight.</t>
-  </si>
-  <si>
-    <t>Content is clearly connected to the topic, is exceptionally insightful, thorough and/or thought provoking and is likely to be of interest to an audience beyond our course.</t>
-  </si>
-  <si>
-    <t>Presentation was engaging, clearly conveyed the project information, used media effectively, allowed equal participation by team members and was an appropriate length.</t>
-  </si>
-  <si>
-    <t>Presentation was not engaging, unclear, incomplete, excessively long or short, used media gratuitously or ineffectively and/or did not balance presentation among team members.</t>
-  </si>
-  <si>
-    <t>Presentation was not engaging, unclear, incomplete, excessively long or short and/or used media gratuitously or ineffectively.</t>
-  </si>
-  <si>
-    <t>Presentation engaging, used media effectively, clearly conveyed the aim, context and plan for the proposed research in an appropriate amount of time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposal was not submitted or is missing significant required content.  </t>
-  </si>
-  <si>
-    <t>The proposal is insufficient and/or unclear in its presentation of the research question and/or literature survey and/or research plan.</t>
-  </si>
-  <si>
-    <t>Proposal clearly states the research question and contextualizes it within the relevant literature and proposes a viable research plan for answering the question..</t>
-  </si>
-  <si>
-    <t>Readings</t>
-  </si>
-  <si>
-    <t>Questions were submitted late, show little thought, miss significant issues, limit or presuppose perspectives or are unlikely to lead to interesting discussion.</t>
-  </si>
-  <si>
-    <t>Questions are thoughtful, probe at the important issues, are open to multiple perspectives  and seem likely to generate interesting discussion.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Questions clearly meet criterion for </t>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> show exceptional potential to illuminate the topic.</t>
+    </r>
+  </si>
+  <si>
+    <t>Written Responses</t>
+  </si>
+  <si>
+    <t>No responses were submitted.</t>
+  </si>
+  <si>
+    <t>Responses were submitted late, show little thought or are poorly written.</t>
+  </si>
+  <si>
+    <t>Limited participation in guiding  discussion, dominated discussion, actively sidetracked discussion, inappropriately stifled voices, was disrespectful and/or demonstrated limited understanding of the issues.</t>
+  </si>
+  <si>
+    <t>No readings were submitted.</t>
+  </si>
+  <si>
+    <t>Readings were submitted late, seem hastily chosen or disconnected from topic, are excessively long or short, miss the academic or current discussion, example or case study.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Readings clearly meet criterion for </t>
     </r>
     <r>
       <rPr>
@@ -1953,69 +1947,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> show exceptional potential to illuminate the topic.</t>
-    </r>
-  </si>
-  <si>
-    <t>Written Responses</t>
-  </si>
-  <si>
-    <t>No responses were submitted.</t>
-  </si>
-  <si>
-    <t>Responses were submitted late, show little thought or are poorly written.</t>
-  </si>
-  <si>
-    <t>Limited participation in guiding  discussion, dominated discussion, actively sidetracked discussion, inappropriately stifled voices, was disrespectful and/or demonstrated limited understanding of the issues.</t>
-  </si>
-  <si>
-    <t>No readings were submitted.</t>
-  </si>
-  <si>
-    <t>Readings were submitted late, seem hastily chosen or disconnected from topic, are excessively long or short, miss the academic or current discussion, example or case study.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Readings clearly meet criterion for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Lucida Grande"/>
-        <family val="2"/>
-      </rPr>
-      <t>✓</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> are exceptionally well suited  to the purpose.</t>
     </r>
   </si>
@@ -2152,34 +2083,40 @@
     <t>On time; One or more reviews may be missing entirely or missing required information; Information in the review does not give an adequate picture of the project; Summaries of each section are cursory or do not align with the review; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
   </si>
   <si>
-    <t>Project Ranking and Selection</t>
-  </si>
-  <si>
-    <t>On time; Wiki contains all required information;  Information presented gives a clear and highly detailed picture of why the team selected the project that they did; Rankings and selection are clearly and well supported by thoughtful, reflective and insightful rationales that draw directly on the gathered information; Writing is clear, concise, well organized, uses complete sentences and proper grammar; Wiki is correctly linked, neatly formatted and easy to read.</t>
-  </si>
-  <si>
-    <t>On time; Wiki contains all required information; Information presented indicates why the team selected the project that they did; Rankings and selection are supported by rationales that mention gathered information; Writing may have minor issues but does not distract from meaning or understanding; Reviews are correctly linked but may be poorly formatted or difficult to read.</t>
-  </si>
-  <si>
-    <t>On time; Wiki may be missing required information; Information in the Wiki does not give an adequate picture of why the team selected the project they did; Rankings may be insufficiently connected to the rationale or rationale may not use or may not align with provided information; Writing, formatting or grammar may interfere with understanding; Reviews may be incorrectly linked, poorly formatted or difficult to read.</t>
-  </si>
-  <si>
-    <t>Blog posts were made on time.</t>
-  </si>
-  <si>
-    <t>Critera</t>
-  </si>
-  <si>
     <t>Blog Post</t>
   </si>
   <si>
-    <t>On time; Post has a thesis that is insightful or will be thought provking and is clearly connected to a course topic; Text integrates readings, discussion and/or other sources; Writing is well organized, gramatically correct. Post is likely to be of interest to an external audience; Links and use of media are integrated and enhance the post; Post is of appropriate length.</t>
-  </si>
-  <si>
     <t>On time; Post has a recognizable thesis and is  connected to a course topic; Text touches on readings, discussion and/or other sources; Writing contains few grammatical errors that do not interfere with meaning; Post may be contextualized in the course, potentially limiting interest to an external audience; Links and use of media may not be fully integrated; Post may be slightly short or long.</t>
   </si>
   <si>
-    <t>On time; Post lacks a thesis and/or is not clearly connected to a course topic; Text does not draw on readings, discussion and/or other sources; Writing is disorganized and/or contains grammatical errors that interfere with meaning; Links and/or use of media seem disconnected or gratuitious; Post is excessively short or long.</t>
+    <t>On time; Post has a thesis that is insightful or will be thought provoking and is clearly connected to a course topic; Text integrates readings, discussion and/or other sources; Writing is well organized, grammatically correct. Post is likely to be of interest to an external audience; Links and use of media are integrated and enhance the post; Post is of appropriate length.</t>
+  </si>
+  <si>
+    <t>On time; Post lacks a thesis and/or is not clearly connected to a course topic; Text does not draw on readings, discussion and/or other sources; Writing is disorganized and/or contains grammatical errors that interfere with meaning; Links and/or use of media seem disconnected or gratuitous; Post is excessively short or long.</t>
+  </si>
+  <si>
+    <t>Project Ranking and Selection Activity</t>
+  </si>
+  <si>
+    <t>Presentation was generally well organized and included all required information; Language, terminology and explanations were generally appropriate to the target audience; Use of media effectively supported the presentation; Participation by individual team member was mildly unbalanced (more or less) as compared to others;  Presentation was  moderately shorter or longer than the target length.</t>
+  </si>
+  <si>
+    <t>Presentation was difficult to follow and/or was missing some required information; Language, terminology and explanations missed the target audience at numerous points; Use of media was ineffective or distracting; Participation by individual team member was moderately to heavily unbalanced (more or less) as compared to others;  Presentation was  significantly shorter or longer than the target length.</t>
+  </si>
+  <si>
+    <t>On time; Wiki contains all required information;  Information presented gives a clear and highly detailed picture of why the team selected the project that they did; Rankings and Selection are clearly and well supported by thoughtful, reflective and insightful rationales that draw directly on the gathered information; Writing is clear, concise, well organized, uses complete sentences and proper grammar; Wiki is correctly linked, neatly formatted and easy to read.</t>
+  </si>
+  <si>
+    <t>On time; Wiki is missing required information; Information in the Wiki does not give an adequate picture of why the team selected the project; Rankings and Selection are insufficiently connected to the rationale or rationale does not use and/or align with provided information; Writing, organization or grammar interferes with understanding; Wiki is incorrectly linked, poorly formatted and/or difficult to read.</t>
+  </si>
+  <si>
+    <t>Presentation was interesting, engaging and told a cohesive story;  All required information was clearly presented in a well organized and easy to follow manner; Language, terminology and explanations were appropriate to the target audience; Use of media (slides, etc.) was visually appealing and enhanced the presentation; Participation was well balanced across team members;  Presentation was at the target length.</t>
+  </si>
+  <si>
+    <t>On time; Wiki contains all required information; Information presented indicates why the team selected the project that they did; Rankings and Selection are supported by rationales that mention gathered information; Writing has minor organizational or grammatical issues that do not distract significantly from meaning or understanding; Wiki is correctly linked but is poorly formatted and/or difficult to read.</t>
+  </si>
+  <si>
+    <t>Presentation was substantially incomplete; Clearly demonstrates little to no investment in the assignment; Individual team member did not participate.</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2243,11 +2180,6 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)_x0000_"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
@@ -2585,7 +2517,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2669,31 +2601,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3166,10 +3107,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
@@ -3183,16 +3124,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="102">
@@ -3200,16 +3141,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="119">
@@ -3217,16 +3158,16 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="86" thickBot="1">
@@ -3234,16 +3175,16 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3277,10 +3218,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="34">
@@ -3288,48 +3229,48 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="102">
       <c r="C5" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="68">
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="86" thickBot="1">
       <c r="C7" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="68">
       <c r="D10" s="9" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="3:5">
@@ -3366,16 +3307,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="3:7" ht="34">
@@ -3383,72 +3324,72 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="120" thickBot="1">
       <c r="C5" s="22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="102">
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="69" thickBot="1">
       <c r="C7" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="102">
       <c r="D10" s="9" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E10" s="9"/>
     </row>
@@ -3490,16 +3431,16 @@
         <v>5</v>
       </c>
       <c r="E11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="51">
@@ -3507,84 +3448,84 @@
         <v>0</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="136">
       <c r="C13" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="136">
       <c r="C14" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="3:8" ht="69" thickBot="1">
       <c r="C15" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="17" thickBot="1">
       <c r="C16" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D16" s="17">
         <v>2</v>
@@ -3636,13 +3577,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="68">
@@ -3650,72 +3591,72 @@
         <v>0</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="119">
       <c r="C13" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="85">
       <c r="C14" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="3:7" ht="69" thickBot="1">
       <c r="C15" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="3:7" ht="17" thickBot="1">
       <c r="C16" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D16" s="17">
         <v>2</v>
@@ -3758,7 +3699,7 @@
   <sheetData>
     <row r="2" spans="3:4" ht="17" thickBot="1">
       <c r="C2" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="17" thickBot="1">
@@ -3766,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="68">
@@ -3774,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="51">
@@ -3782,7 +3723,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="68">
@@ -3790,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="35" thickBot="1">
@@ -3798,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3816,15 +3757,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
   <dimension ref="C2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="4" max="5" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="17" thickBot="1"/>
@@ -3833,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="3:6" ht="102">
@@ -3841,7 +3781,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="F4" s="37"/>
     </row>
@@ -3850,7 +3790,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="F5" s="37"/>
     </row>
@@ -3859,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="52" thickBot="1">
@@ -3867,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="17" thickBot="1"/>
@@ -3876,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="119">
@@ -3884,7 +3824,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="119">
@@ -3892,7 +3832,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="3:6" ht="136">
@@ -3900,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="52" thickBot="1">
@@ -3908,48 +3848,63 @@
         <v>0</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" ht="17" thickBot="1"/>
-    <row r="21" spans="3:4" ht="17" thickBot="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="17" thickBot="1"/>
+    <row r="21" spans="3:5" ht="17" thickBot="1">
       <c r="C21" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" ht="153">
+      <c r="D21" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="153">
       <c r="C22" s="35">
         <v>3</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" ht="116" customHeight="1">
+      <c r="D22" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="136">
       <c r="C23" s="33">
         <v>2</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" ht="132" customHeight="1">
+      <c r="D23" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="132" customHeight="1">
       <c r="C24" s="33">
         <v>1</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" ht="52" thickBot="1">
+      <c r="D24" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="52" thickBot="1">
       <c r="C25" s="32">
         <v>0</v>
       </c>
-      <c r="D25" s="34" t="s">
-        <v>214</v>
+      <c r="D25" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3960,10 +3915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3973,189 +3928,54 @@
     <col min="9" max="12" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17" thickBot="1"/>
-    <row r="2" spans="2:12" ht="17" thickBot="1">
+    <row r="1" spans="2:3" ht="17" thickBot="1"/>
+    <row r="2" spans="2:3" ht="17" thickBot="1">
       <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="137" thickBot="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="137" thickBot="1">
       <c r="B3" s="35">
         <v>3</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="154" thickBot="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="154" thickBot="1">
       <c r="B4" s="33">
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="121" customHeight="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="121" customHeight="1">
       <c r="B5" s="33">
         <v>1</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="52" thickBot="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="52" thickBot="1">
       <c r="B6" s="32">
         <v>0</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="17" customHeight="1"/>
-    <row r="9" spans="2:12" ht="17" thickBot="1"/>
-    <row r="10" spans="2:12" ht="17" thickBot="1">
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="17" customHeight="1"/>
+    <row r="8" spans="2:3" ht="204">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="103" thickBot="1">
-      <c r="H11" s="22">
-        <v>3</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="102">
-      <c r="H12" s="21">
-        <v>2</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="86" thickBot="1">
-      <c r="H13" s="22">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="51">
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="85">
-      <c r="I16" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9">
-      <c r="I17" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="8:9" ht="17" thickBot="1"/>
-    <row r="21" spans="8:9" ht="17" thickBot="1">
-      <c r="H21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="8:9" ht="18" thickBot="1">
-      <c r="H22" s="22">
-        <v>3</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="8:9" ht="17">
-      <c r="H23" s="21">
-        <v>2</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="8:9" ht="18" thickBot="1">
-      <c r="H24" s="22">
-        <v>1</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="8:9" ht="34">
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>99</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I17" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -4182,8 +4002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="D3:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4198,16 +4018,16 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="4:8" ht="51">
@@ -4215,67 +4035,67 @@
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="4:8" ht="103" thickBot="1">
       <c r="D6" s="22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="4:8" ht="102">
       <c r="D7" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="4:8" ht="69" thickBot="1">
       <c r="D8" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="4:8" ht="17" thickBot="1"/>
@@ -4284,16 +4104,16 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="4:8" ht="51">
@@ -4301,67 +4121,67 @@
         <v>0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="4:8" ht="86" thickBot="1">
       <c r="D14" s="22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="4:8" ht="102">
       <c r="D15" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="4:8" ht="69" thickBot="1">
       <c r="D16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="H16" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4395,22 +4215,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="3:9" ht="51">
@@ -4418,91 +4238,91 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="103" thickBot="1">
       <c r="C5" s="22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="85">
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:9" ht="86" thickBot="1">
       <c r="C7" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4551,19 +4371,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="68">
@@ -4571,64 +4391,64 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="3:8" ht="117" customHeight="1">
       <c r="C5" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="102">
       <c r="C6" s="21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="69" thickBot="1">
       <c r="C7" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>4</v>
@@ -4637,18 +4457,18 @@
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="119">
       <c r="E9" s="9" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="3:8">

</xml_diff>

<commit_message>
Added Tech Spike assignment; Adjusted schedule
</commit_message>
<xml_diff>
--- a/docs/Rubrics.xlsx
+++ b/docs/Rubrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braught/courses/Fall22/COMP491/website/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55989D03-64EC-274A-9E9C-13779BF4AF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D028E13-7A07-1D44-A9EA-4FE57C4CC6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3200" yWindow="-21040" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3200" yWindow="-21040" windowWidth="26820" windowHeight="17720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAE" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="ProjSelection" sheetId="24" r:id="rId3"/>
     <sheet name="Blog" sheetId="3" r:id="rId4"/>
     <sheet name="BugGardening" sheetId="25" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="22" r:id="rId6"/>
-    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId7"/>
-    <sheet name="ProjectCheckpoint" sheetId="4" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="23" r:id="rId9"/>
-    <sheet name="Poster" sheetId="21" r:id="rId10"/>
-    <sheet name="CodeReview" sheetId="19" r:id="rId11"/>
-    <sheet name="Discussion" sheetId="18" r:id="rId12"/>
-    <sheet name="ProjectReport" sheetId="15" r:id="rId13"/>
-    <sheet name="ResearchReport" sheetId="17" r:id="rId14"/>
+    <sheet name="Tech Spike" sheetId="26" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="22" r:id="rId7"/>
+    <sheet name="ProjSel-ResearchProp" sheetId="12" r:id="rId8"/>
+    <sheet name="ProjectCheckpoint" sheetId="4" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId10"/>
+    <sheet name="Poster" sheetId="21" r:id="rId11"/>
+    <sheet name="CodeReview" sheetId="19" r:id="rId12"/>
+    <sheet name="Discussion" sheetId="18" r:id="rId13"/>
+    <sheet name="ProjectReport" sheetId="15" r:id="rId14"/>
+    <sheet name="ResearchReport" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="227">
   <si>
     <t>Score</t>
   </si>
@@ -2130,6 +2131,33 @@
   </si>
   <si>
     <t>On time; Project's bug information is incomplete or insufficiently detailed.  Individual did not report on required number of suspect bugs;  Individual's suspect issue reports are incomplete, missing live links, and lack sufficient detail; Reasonable action was not taken on any suspect issue. Wiki page has organization and/or formatting issues.</t>
+  </si>
+  <si>
+    <t>Presentation was interesting, engaging and told a cohesive story;  All required information was clearly presented in a well organized and easy to follow manner; Language, terminology and explanations were appropriate to the target audience; Use of media (slides, etc.) was visually appealing and enhanced the presentation; Demonstration provided clear and compelling evidence of substantial learning; Participation was well balanced across team members;  Presentation was at the target length.</t>
+  </si>
+  <si>
+    <t>Presentation was generally well organized and included all required information; Language, terminology and explanations were generally appropriate to the target audience; Use of media effectively supported the presentation; Demonstration provided evidence of learning; Participation by individual team member was mildly unbalanced (more or less) as compared to others;  Presentation was  moderately shorter or longer than the target length.</t>
+  </si>
+  <si>
+    <t>Presentation was substantially incomplete; Clearly demonstrates little to no investment in the assignment; No demonstration was given; Individual team member did not participate.</t>
+  </si>
+  <si>
+    <t>Gap Analysis &amp; Learning Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On time; Gap analysis is detailed and thoughtful about the project demands and the team members' knowledge and skills; Learning resources are well selected and detailed annotations are given; Wiki contains all required information, is correctly linked, neatly formatted and easy to read;  Writing is clear, concise, well organized, uses complete sentences and proper grammar; Individual's contributions to Live-Logs are detailed and clearly demonstrate sufficient, regular and sustained time and effort. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On time; Gap analysis is complete; Learning resources seem appropriate and are annotated; Wiki contains all required information, is correctly linked but formatting may distract from readability; Writing has minor organizational or grammatical issues that do not distract significantly from meaning or understanding; Individual's contributions to Live-Logs demonstrate some investment of time and effort. </t>
+  </si>
+  <si>
+    <t>On time; Gap analysis is cursory or missing information; Learning resources are not well suited to learning goals, team members or timeframe, and/or lack meaningful annotations; Wiki is missing required information, incorrectly linked, poorly formatted and/or difficult to read; Writing, organization or grammar interferes with understanding; Individual's contributions (or lack there of) to Live-Logs demonstrate insufficient investment of time and effort.</t>
+  </si>
+  <si>
+    <t>Presentation was difficult to follow and/or was missing some required information; Language, terminology and explanations missed the target audience at numerous points; Use of media was ineffective or distracting; Demonstration did not provide evidence of sufficient learning;  Participation by individual team member was moderately to heavily unbalanced (more or less) as compared to others;  Presentation was  significantly shorter or longer than the target length.</t>
+  </si>
+  <si>
+    <t>Late, missing or substantially incomplete; Clearly demonstrates little to no investment in the assignment. Individual's lack of contributions to Live-Logs  demonstrate no investment of time and effort.</t>
   </si>
 </sst>
 </file>
@@ -3212,6 +3240,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B90E7E3-D2D8-464A-A6B2-25D7F2B455CA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:H10"/>
   <sheetViews>
@@ -3348,7 +3388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:E11"/>
   <sheetViews>
@@ -3437,7 +3477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:G11"/>
   <sheetViews>
@@ -3558,7 +3598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C10:H16"/>
   <sheetViews>
@@ -3704,7 +3744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="C10:G16"/>
   <sheetViews>
@@ -3907,8 +3947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C29E0-82A2-5449-9321-281A08D7D7C2}">
   <dimension ref="C2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4024,7 +4064,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="3:5" ht="153">
+    <row r="23" spans="3:5" ht="136">
       <c r="C23" s="33">
         <v>2</v>
       </c>
@@ -4140,7 +4180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796DAA43-8A15-054F-BD9C-8FB9E4206D17}">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -4168,7 +4208,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="120" thickBot="1">
+    <row r="4" spans="2:3" ht="137" thickBot="1">
       <c r="B4" s="33">
         <v>2</v>
       </c>
@@ -4203,6 +4243,81 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B73619E-924E-CF41-BB65-0DE45B27F9CC}">
+  <dimension ref="B3:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C8" sqref="C4:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="4" width="47.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="17" thickBot="1"/>
+    <row r="4" spans="2:4" ht="17" thickBot="1">
+      <c r="B4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="170">
+      <c r="B5" s="35">
+        <v>3</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="153">
+      <c r="B6" s="33">
+        <v>2</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="161" customHeight="1">
+      <c r="B7" s="33">
+        <v>1</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="69" thickBot="1">
+      <c r="B8" s="32">
+        <v>0</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB29A2B-D501-E842-859E-32CF9B172168}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4214,7 +4329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="D3:H16"/>
   <sheetViews>
@@ -4411,7 +4526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C2:I7"/>
   <sheetViews>
@@ -4550,16 +4665,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B90E7E3-D2D8-464A-A6B2-25D7F2B455CA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>